<commit_message>
Partial implementation of sponsor contracts.
</commit_message>
<xml_diff>
--- a/WorkingNotes/research.xlsx
+++ b/WorkingNotes/research.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\GpwEditor\WorkingNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E80E61A-7B54-44AB-ABFA-AE03B5E869CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="576">
   <si>
     <t>7E9FC0</t>
   </si>
@@ -1732,12 +1734,33 @@
   </si>
   <si>
     <t>TeamId -1 * 4</t>
+  </si>
+  <si>
+    <t>120526C</t>
+  </si>
+  <si>
+    <t>Auto Motor Sport</t>
+  </si>
+  <si>
+    <t>Castrol</t>
+  </si>
+  <si>
+    <t>Falke</t>
+  </si>
+  <si>
+    <t>Komatsu</t>
+  </si>
+  <si>
+    <t>Sonax</t>
+  </si>
+  <si>
+    <t>Universal Studios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2110,7 +2133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5742,10 +5765,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6557,43 +6582,43 @@
         <v>35</v>
       </c>
       <c r="E15" s="10">
-        <f>HEX2DEC(E3)-HEX2DEC(E2)</f>
+        <f t="shared" ref="E15:N15" si="1">HEX2DEC(E3)-HEX2DEC(E2)</f>
         <v>7824</v>
       </c>
       <c r="F15" s="10">
-        <f>HEX2DEC(F3)-HEX2DEC(F2)</f>
+        <f t="shared" si="1"/>
         <v>7808</v>
       </c>
       <c r="G15" s="10">
-        <f>HEX2DEC(G3)-HEX2DEC(G2)</f>
+        <f t="shared" si="1"/>
         <v>7824</v>
       </c>
       <c r="H15" s="10">
-        <f>HEX2DEC(H3)-HEX2DEC(H2)</f>
+        <f t="shared" si="1"/>
         <v>7804</v>
       </c>
       <c r="I15" s="10">
-        <f>HEX2DEC(I3)-HEX2DEC(I2)</f>
+        <f t="shared" si="1"/>
         <v>7824</v>
       </c>
       <c r="J15" s="10">
-        <f>HEX2DEC(J3)-HEX2DEC(J2)</f>
+        <f t="shared" si="1"/>
         <v>7828</v>
       </c>
       <c r="K15" s="10">
-        <f>HEX2DEC(K3)-HEX2DEC(K2)</f>
+        <f t="shared" si="1"/>
         <v>7824</v>
       </c>
       <c r="L15" s="10">
-        <f>HEX2DEC(L3)-HEX2DEC(L2)</f>
+        <f t="shared" si="1"/>
         <v>7824</v>
       </c>
       <c r="M15" s="10">
-        <f>HEX2DEC(M3)-HEX2DEC(M2)</f>
+        <f t="shared" si="1"/>
         <v>7824</v>
       </c>
       <c r="N15" s="10">
-        <f>HEX2DEC(N3)-HEX2DEC(N2)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R15" s="10">
@@ -6617,43 +6642,43 @@
         <v>75</v>
       </c>
       <c r="E16" s="10">
-        <f t="shared" ref="E16:F24" si="1">HEX2DEC(E4)-HEX2DEC(E3)</f>
+        <f t="shared" ref="E16:F24" si="2">HEX2DEC(E4)-HEX2DEC(E3)</f>
         <v>7824</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7828</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" ref="G16:H16" si="2">HEX2DEC(G4)-HEX2DEC(G3)</f>
+        <f t="shared" ref="G16:H16" si="3">HEX2DEC(G4)-HEX2DEC(G3)</f>
         <v>7824</v>
       </c>
       <c r="H16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7844</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" ref="I16:J16" si="3">HEX2DEC(I4)-HEX2DEC(I3)</f>
+        <f t="shared" ref="I16:J16" si="4">HEX2DEC(I4)-HEX2DEC(I3)</f>
         <v>7824</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7828</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" ref="K16:N16" si="4">HEX2DEC(K4)-HEX2DEC(K3)</f>
+        <f t="shared" ref="K16:N16" si="5">HEX2DEC(K4)-HEX2DEC(K3)</f>
         <v>7824</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7820</v>
       </c>
       <c r="M16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7824</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R16" s="10">
@@ -6677,43 +6702,43 @@
         <v>71</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7832</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" ref="G17:H17" si="5">HEX2DEC(G5)-HEX2DEC(G4)</f>
+        <f t="shared" ref="G17:H17" si="6">HEX2DEC(G5)-HEX2DEC(G4)</f>
         <v>7824</v>
       </c>
       <c r="H17" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7812</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" ref="I17:J17" si="6">HEX2DEC(I5)-HEX2DEC(I4)</f>
+        <f t="shared" ref="I17:J17" si="7">HEX2DEC(I5)-HEX2DEC(I4)</f>
         <v>7824</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7828</v>
       </c>
       <c r="K17" s="10">
-        <f t="shared" ref="K17:N17" si="7">HEX2DEC(K5)-HEX2DEC(K4)</f>
+        <f t="shared" ref="K17:N17" si="8">HEX2DEC(K5)-HEX2DEC(K4)</f>
         <v>7824</v>
       </c>
       <c r="L17" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7824</v>
       </c>
       <c r="M17" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7824</v>
       </c>
       <c r="N17" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="R17" s="10">
@@ -6737,43 +6762,43 @@
         <v>72</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7804</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" ref="G18:H18" si="8">HEX2DEC(G6)-HEX2DEC(G5)</f>
+        <f t="shared" ref="G18:H18" si="9">HEX2DEC(G6)-HEX2DEC(G5)</f>
         <v>7824</v>
       </c>
       <c r="H18" s="10">
-        <f t="shared" si="8"/>
-        <v>7828</v>
-      </c>
-      <c r="I18" s="10">
-        <f t="shared" ref="I18:J18" si="9">HEX2DEC(I6)-HEX2DEC(I5)</f>
-        <v>7824</v>
-      </c>
-      <c r="J18" s="10">
         <f t="shared" si="9"/>
         <v>7828</v>
       </c>
-      <c r="K18" s="10">
-        <f t="shared" ref="K18:N18" si="10">HEX2DEC(K6)-HEX2DEC(K5)</f>
-        <v>7824</v>
-      </c>
-      <c r="L18" s="10">
+      <c r="I18" s="10">
+        <f t="shared" ref="I18:J18" si="10">HEX2DEC(I6)-HEX2DEC(I5)</f>
+        <v>7824</v>
+      </c>
+      <c r="J18" s="10">
         <f t="shared" si="10"/>
         <v>7828</v>
       </c>
+      <c r="K18" s="10">
+        <f t="shared" ref="K18:N18" si="11">HEX2DEC(K6)-HEX2DEC(K5)</f>
+        <v>7824</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="11"/>
+        <v>7828</v>
+      </c>
       <c r="M18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7824</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="R18" s="10">
@@ -6797,43 +6822,43 @@
         <v>73</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7828</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" ref="G19:H19" si="11">HEX2DEC(G7)-HEX2DEC(G6)</f>
+        <f t="shared" ref="G19:H19" si="12">HEX2DEC(G7)-HEX2DEC(G6)</f>
         <v>7824</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" si="11"/>
-        <v>7828</v>
-      </c>
-      <c r="I19" s="10">
-        <f t="shared" ref="I19:J19" si="12">HEX2DEC(I7)-HEX2DEC(I6)</f>
-        <v>7824</v>
-      </c>
-      <c r="J19" s="10">
         <f t="shared" si="12"/>
         <v>7828</v>
       </c>
+      <c r="I19" s="10">
+        <f t="shared" ref="I19:J19" si="13">HEX2DEC(I7)-HEX2DEC(I6)</f>
+        <v>7824</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="13"/>
+        <v>7828</v>
+      </c>
       <c r="K19" s="10">
-        <f t="shared" ref="K19:N19" si="13">HEX2DEC(K7)-HEX2DEC(K6)</f>
+        <f t="shared" ref="K19:N19" si="14">HEX2DEC(K7)-HEX2DEC(K6)</f>
         <v>7824</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7820</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7824</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="R19" s="10">
@@ -6857,43 +6882,43 @@
         <v>36</v>
       </c>
       <c r="E20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7836</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" ref="G20:H20" si="14">HEX2DEC(G8)-HEX2DEC(G7)</f>
+        <f t="shared" ref="G20:H20" si="15">HEX2DEC(G8)-HEX2DEC(G7)</f>
         <v>7824</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" si="14"/>
-        <v>7808</v>
-      </c>
-      <c r="I20" s="10">
-        <f t="shared" ref="I20:J20" si="15">HEX2DEC(I8)-HEX2DEC(I7)</f>
-        <v>7824</v>
-      </c>
-      <c r="J20" s="10">
         <f t="shared" si="15"/>
         <v>7808</v>
       </c>
+      <c r="I20" s="10">
+        <f t="shared" ref="I20:J20" si="16">HEX2DEC(I8)-HEX2DEC(I7)</f>
+        <v>7824</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="16"/>
+        <v>7808</v>
+      </c>
       <c r="K20" s="10">
-        <f t="shared" ref="K20:N20" si="16">HEX2DEC(K8)-HEX2DEC(K7)</f>
+        <f t="shared" ref="K20:N20" si="17">HEX2DEC(K8)-HEX2DEC(K7)</f>
         <v>7824</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7828</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7824</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="R20" s="10">
@@ -6917,43 +6942,43 @@
         <v>34</v>
       </c>
       <c r="E21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7920</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" ref="G21:H21" si="17">HEX2DEC(G9)-HEX2DEC(G8)</f>
+        <f t="shared" ref="G21:H21" si="18">HEX2DEC(G9)-HEX2DEC(G8)</f>
         <v>7824</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7820</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" ref="I21:J21" si="18">HEX2DEC(I9)-HEX2DEC(I8)</f>
+        <f t="shared" ref="I21:J21" si="19">HEX2DEC(I9)-HEX2DEC(I8)</f>
         <v>7824</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7844</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" ref="K21:N21" si="19">HEX2DEC(K9)-HEX2DEC(K8)</f>
+        <f t="shared" ref="K21:N21" si="20">HEX2DEC(K9)-HEX2DEC(K8)</f>
         <v>7824</v>
       </c>
       <c r="L21" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7820</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7824</v>
       </c>
       <c r="N21" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="R21" s="10">
@@ -6977,43 +7002,43 @@
         <v>46</v>
       </c>
       <c r="E22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8024</v>
       </c>
       <c r="G22" s="10">
-        <f t="shared" ref="G22:H22" si="20">HEX2DEC(G10)-HEX2DEC(G9)</f>
+        <f t="shared" ref="G22:H22" si="21">HEX2DEC(G10)-HEX2DEC(G9)</f>
         <v>7824</v>
       </c>
       <c r="H22" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7832</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" ref="I22:J22" si="21">HEX2DEC(I10)-HEX2DEC(I9)</f>
+        <f t="shared" ref="I22:J22" si="22">HEX2DEC(I10)-HEX2DEC(I9)</f>
         <v>7824</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7828</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" ref="K22:N22" si="22">HEX2DEC(K10)-HEX2DEC(K9)</f>
+        <f t="shared" ref="K22:N22" si="23">HEX2DEC(K10)-HEX2DEC(K9)</f>
         <v>7824</v>
       </c>
       <c r="L22" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7824</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7824</v>
       </c>
       <c r="N22" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="R22" s="10">
@@ -7037,43 +7062,43 @@
         <v>47</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7852</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" ref="G23:H23" si="23">HEX2DEC(G11)-HEX2DEC(G10)</f>
+        <f t="shared" ref="G23:H23" si="24">HEX2DEC(G11)-HEX2DEC(G10)</f>
         <v>7824</v>
       </c>
       <c r="H23" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>7824</v>
       </c>
       <c r="I23" s="10">
-        <f t="shared" ref="I23:J23" si="24">HEX2DEC(I11)-HEX2DEC(I10)</f>
+        <f t="shared" ref="I23:J23" si="25">HEX2DEC(I11)-HEX2DEC(I10)</f>
         <v>7824</v>
       </c>
       <c r="J23" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7820</v>
       </c>
       <c r="K23" s="10">
-        <f t="shared" ref="K23:N23" si="25">HEX2DEC(K11)-HEX2DEC(K10)</f>
+        <f t="shared" ref="K23:N23" si="26">HEX2DEC(K11)-HEX2DEC(K10)</f>
         <v>7824</v>
       </c>
       <c r="L23" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>7828</v>
       </c>
       <c r="M23" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>7824</v>
       </c>
       <c r="N23" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>4</v>
       </c>
       <c r="R23" s="10">
@@ -7091,43 +7116,43 @@
         <v>48</v>
       </c>
       <c r="E24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7824</v>
       </c>
       <c r="F24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7716</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" ref="G24:H24" si="26">HEX2DEC(G12)-HEX2DEC(G11)</f>
+        <f t="shared" ref="G24:H24" si="27">HEX2DEC(G12)-HEX2DEC(G11)</f>
         <v>7824</v>
       </c>
       <c r="H24" s="10">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>7824</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" ref="I24:J24" si="27">HEX2DEC(I12)-HEX2DEC(I11)</f>
+        <f t="shared" ref="I24:J24" si="28">HEX2DEC(I12)-HEX2DEC(I11)</f>
         <v>7824</v>
       </c>
       <c r="J24" s="10">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>7824</v>
       </c>
       <c r="K24" s="10">
-        <f t="shared" ref="K24:N24" si="28">HEX2DEC(K12)-HEX2DEC(K11)</f>
+        <f t="shared" ref="K24:N24" si="29">HEX2DEC(K12)-HEX2DEC(K11)</f>
         <v>7824</v>
       </c>
       <c r="L24" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7820</v>
       </c>
       <c r="M24" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7824</v>
       </c>
       <c r="N24" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="R24" s="10">
@@ -7227,36 +7252,36 @@
         <v>551</v>
       </c>
       <c r="F27" s="10">
-        <f t="shared" ref="F27:H36" si="29">HEX2DEC(F3)-HEX2DEC($E3)</f>
+        <f t="shared" ref="F27:H36" si="30">HEX2DEC(F3)-HEX2DEC($E3)</f>
         <v>316</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>352</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>185</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" ref="J27:N27" si="30">HEX2DEC(J3)-HEX2DEC($E3)</f>
+        <f t="shared" ref="J27:M27" si="31">HEX2DEC(J3)-HEX2DEC($E3)</f>
         <v>384</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>175</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>340</v>
       </c>
       <c r="M27" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>700</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" ref="N27:N36" si="31">HEX2DEC(N3)-HEX2DEC($E$2)</f>
+        <f t="shared" ref="N27:N36" si="32">HEX2DEC(N3)-HEX2DEC($E$2)</f>
         <v>-8638468</v>
       </c>
       <c r="R27" s="10">
@@ -7283,36 +7308,36 @@
         <v>170</v>
       </c>
       <c r="F28" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>320</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>182</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>372</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>186</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" ref="J28:N28" si="32">HEX2DEC(J4)-HEX2DEC($E4)</f>
+        <f t="shared" ref="J28:M28" si="33">HEX2DEC(J4)-HEX2DEC($E4)</f>
         <v>388</v>
       </c>
       <c r="K28" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L28" s="10">
+        <f t="shared" si="33"/>
+        <v>336</v>
+      </c>
+      <c r="M28" s="10">
+        <f t="shared" si="33"/>
+        <v>700</v>
+      </c>
+      <c r="N28" s="10">
         <f t="shared" si="32"/>
-        <v>336</v>
-      </c>
-      <c r="M28" s="10">
-        <f t="shared" si="32"/>
-        <v>700</v>
-      </c>
-      <c r="N28" s="10">
-        <f t="shared" si="31"/>
         <v>-8638464</v>
       </c>
       <c r="R28" s="10">
@@ -7339,36 +7364,36 @@
         <v>172</v>
       </c>
       <c r="F29" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>328</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>547</v>
       </c>
       <c r="H29" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>360</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>187</v>
       </c>
       <c r="J29" s="10">
-        <f t="shared" ref="J29:N29" si="33">HEX2DEC(J5)-HEX2DEC($E5)</f>
+        <f t="shared" ref="J29:M29" si="34">HEX2DEC(J5)-HEX2DEC($E5)</f>
         <v>392</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L29" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>336</v>
       </c>
       <c r="M29" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>700</v>
       </c>
       <c r="N29" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638460</v>
       </c>
       <c r="R29" s="10">
@@ -7395,36 +7420,36 @@
         <v>550</v>
       </c>
       <c r="F30" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>308</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>549</v>
       </c>
       <c r="H30" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>364</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>188</v>
       </c>
       <c r="J30" s="10">
-        <f t="shared" ref="J30:N30" si="34">HEX2DEC(J6)-HEX2DEC($E6)</f>
+        <f t="shared" ref="J30:M30" si="35">HEX2DEC(J6)-HEX2DEC($E6)</f>
         <v>396</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>175</v>
       </c>
       <c r="L30" s="10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>340</v>
       </c>
       <c r="M30" s="10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>700</v>
       </c>
       <c r="N30" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638456</v>
       </c>
       <c r="R30" s="10">
@@ -7451,36 +7476,36 @@
         <v>168</v>
       </c>
       <c r="F31" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>312</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>181</v>
       </c>
       <c r="H31" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>368</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>189</v>
       </c>
       <c r="J31" s="10">
-        <f t="shared" ref="J31:N31" si="35">HEX2DEC(J7)-HEX2DEC($E7)</f>
+        <f t="shared" ref="J31:M31" si="36">HEX2DEC(J7)-HEX2DEC($E7)</f>
         <v>400</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L31" s="10">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>336</v>
       </c>
       <c r="M31" s="10">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>700</v>
       </c>
       <c r="N31" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638452</v>
       </c>
       <c r="R31" s="10">
@@ -7507,36 +7532,36 @@
         <v>171</v>
       </c>
       <c r="F32" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>324</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>35</v>
       </c>
       <c r="H32" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>352</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>185</v>
       </c>
       <c r="J32" s="10">
-        <f t="shared" ref="J32:N32" si="36">HEX2DEC(J8)-HEX2DEC($E8)</f>
+        <f t="shared" ref="J32:M32" si="37">HEX2DEC(J8)-HEX2DEC($E8)</f>
         <v>384</v>
       </c>
       <c r="K32" s="10" t="s">
         <v>175</v>
       </c>
       <c r="L32" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>340</v>
       </c>
       <c r="M32" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>700</v>
       </c>
       <c r="N32" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638448</v>
       </c>
       <c r="R32" s="10">
@@ -7563,36 +7588,36 @@
         <v>194</v>
       </c>
       <c r="F33" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>420</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>177</v>
       </c>
       <c r="H33" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>348</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>190</v>
       </c>
       <c r="J33" s="10">
-        <f t="shared" ref="J33:N33" si="37">HEX2DEC(J9)-HEX2DEC($E9)</f>
+        <f t="shared" ref="J33:M33" si="38">HEX2DEC(J9)-HEX2DEC($E9)</f>
         <v>404</v>
       </c>
       <c r="K33" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L33" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>336</v>
       </c>
       <c r="M33" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>700</v>
       </c>
       <c r="N33" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638444</v>
       </c>
       <c r="R33" s="10">
@@ -7619,36 +7644,36 @@
         <v>552</v>
       </c>
       <c r="F34" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>620</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>178</v>
       </c>
       <c r="H34" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>356</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>191</v>
       </c>
       <c r="J34" s="10">
-        <f t="shared" ref="J34:N34" si="38">HEX2DEC(J10)-HEX2DEC($E10)</f>
+        <f t="shared" ref="J34:M34" si="39">HEX2DEC(J10)-HEX2DEC($E10)</f>
         <v>408</v>
       </c>
       <c r="K34" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L34" s="10">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>336</v>
       </c>
       <c r="M34" s="10">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>700</v>
       </c>
       <c r="N34" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638440</v>
       </c>
       <c r="R34" s="10">
@@ -7675,36 +7700,36 @@
         <v>553</v>
       </c>
       <c r="F35" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>648</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>178</v>
       </c>
       <c r="H35" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>356</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>190</v>
       </c>
       <c r="J35" s="10">
-        <f t="shared" ref="J35:N35" si="39">HEX2DEC(J11)-HEX2DEC($E11)</f>
+        <f t="shared" ref="J35:M35" si="40">HEX2DEC(J11)-HEX2DEC($E11)</f>
         <v>404</v>
       </c>
       <c r="K35" s="10" t="s">
         <v>175</v>
       </c>
       <c r="L35" s="10">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>340</v>
       </c>
       <c r="M35" s="10">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>700</v>
       </c>
       <c r="N35" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638436</v>
       </c>
     </row>
@@ -7722,36 +7747,36 @@
         <v>554</v>
       </c>
       <c r="F36" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>540</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>178</v>
       </c>
       <c r="H36" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>356</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>190</v>
       </c>
       <c r="J36" s="10">
-        <f t="shared" ref="J36:N36" si="40">HEX2DEC(J12)-HEX2DEC($E12)</f>
+        <f t="shared" ref="J36:M36" si="41">HEX2DEC(J12)-HEX2DEC($E12)</f>
         <v>404</v>
       </c>
       <c r="K36" s="10" t="s">
         <v>174</v>
       </c>
       <c r="L36" s="10">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>336</v>
       </c>
       <c r="M36" s="10">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>700</v>
       </c>
       <c r="N36" s="10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>-8638432</v>
       </c>
     </row>
@@ -9498,4 +9523,184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA8644C-41AD-4A54-BCE8-1C7AF19E30AC}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1">
+        <f>HEX2DEC(A1)-HEX2DEC(A$12)</f>
+        <v>28</v>
+      </c>
+      <c r="C1">
+        <f>B1/4</f>
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B10" si="0">HEX2DEC(A2)-HEX2DEC(A$12)</f>
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C10" si="1">B2/4</f>
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>372</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>376</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>569</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further implementation of sponsor entity and sponsor contract support. Checking in prior to clean up.
</commit_message>
<xml_diff>
--- a/WorkingNotes/research.xlsx
+++ b/WorkingNotes/research.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\GpwEditor\WorkingNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E80E61A-7B54-44AB-ABFA-AE03B5E869CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A279B8-2177-4D42-B597-1DD075014932}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="684">
   <si>
     <t>7E9FC0</t>
   </si>
@@ -1755,6 +1755,330 @@
   </si>
   <si>
     <t>Universal Studios</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1209364, 2   // Tyre Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1209338, 2   // Tyre Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1F4, 3   // Tyre McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1C8, 3   // Tyre McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EF14, 1   // Tyre Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EEE8, 0   // Tyre Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C34, 1   // Tyre Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C08, 0   // Tyre Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214AC4, 1   // Tyre Stewart</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214A98, 0   // Tyre Stewart</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187E4, 1   // Tyre Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187B8, 0   // Tyre Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1205644, 2   // Tyre Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1205618, 3   // Tyre Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074D4, 3   // Tyre Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074A8, 3   // Tyre Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D084, 1   // Tyre Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D058, 0   // Tyre Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210DA4, 1   // Tyre Sauber</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210D78, 0   // Tyre Sauber</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1216954, 1   // Tyre Tyrrell</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1216928, 0   // Tyre Tyrrell</t>
+  </si>
+  <si>
+    <t>0120B1F4</t>
+  </si>
+  <si>
+    <t>0120B1C8</t>
+  </si>
+  <si>
+    <t>0120EF14</t>
+  </si>
+  <si>
+    <t>0120EEE8</t>
+  </si>
+  <si>
+    <t>01212C34</t>
+  </si>
+  <si>
+    <t>01212C08</t>
+  </si>
+  <si>
+    <t>01214AC4</t>
+  </si>
+  <si>
+    <t>01214A98</t>
+  </si>
+  <si>
+    <t>012187B8</t>
+  </si>
+  <si>
+    <t>012074D4</t>
+  </si>
+  <si>
+    <t>012074A8</t>
+  </si>
+  <si>
+    <t>0120D084</t>
+  </si>
+  <si>
+    <t>0120D058</t>
+  </si>
+  <si>
+    <t>01210DA4</t>
+  </si>
+  <si>
+    <t>01210D78</t>
+  </si>
+  <si>
+    <t>12187E4</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C30, 1   // Engine Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C04, 0   // Engine Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074D0, 3   // Engine Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074A4, 3   // Engine Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210DA0, 1   // Engine Sauber</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210D74, 0   // Engine Sauber</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214AC0, 3   // Engine Stewart</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214A94, 2   // Engine Stewart</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1216950, 1   // Engine Tyrrell</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1216924, 0   // Engine Tyrrell</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187E0, 1   // Engine Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187B4, 0   // Engine Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1F0, 3   // Engine McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1C4, 3   // Engine McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D080, 2   // Engine Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D054, 2   // Engine Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EF10, 3   // Engine Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EEE4, 2   // Engine Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1205640, 1   // Engine Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1205614, 0   // Engine Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1209360, 1   // Engine Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1209334, 0   // Engine Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1205648, 1   // Fuel Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120561C, 0   // Fuel Williams</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074D8, 3   // Fuel Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12074AC, 3   // Fuel Ferrari</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1209368, 2   // Fuel Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120933C, 2   // Fuel Benetton</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1F8, 3   // Fuel McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120B1CC, 3   // Fuel McLaren</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D088, 2   // Fuel Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120D05C, 2   // Fuel Jordan</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EF18, 2   // Fuel Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_120EEEC, 3   // Fuel Prost</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C38, 2   // Fuel Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1212C0C, 3   // Fuel Arrows</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187E8, 1   // Fuel Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_12187BC, 0   // Fuel Minardi</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1216958, 1   // Fuel Tyrrell</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_121692C, 0   // Fuel Tyrrell</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214AC8, 2   // Fuel Stewart</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1214A9C, 2   // Fuel Stewart</t>
+  </si>
+  <si>
+    <t>120561C</t>
+  </si>
+  <si>
+    <t>12074D8</t>
+  </si>
+  <si>
+    <t>12074AC</t>
+  </si>
+  <si>
+    <t>1210DA8</t>
+  </si>
+  <si>
+    <t>1210D7C</t>
+  </si>
+  <si>
+    <t>120933C</t>
+  </si>
+  <si>
+    <t>120B1F8</t>
+  </si>
+  <si>
+    <t>120B1CC</t>
+  </si>
+  <si>
+    <t>120D088</t>
+  </si>
+  <si>
+    <t>120D05C</t>
+  </si>
+  <si>
+    <t>120EF18</t>
+  </si>
+  <si>
+    <t>1212C38</t>
+  </si>
+  <si>
+    <t>1212C0C</t>
+  </si>
+  <si>
+    <t>12187BC</t>
+  </si>
+  <si>
+    <t>121692C</t>
+  </si>
+  <si>
+    <t>1214AC8</t>
+  </si>
+  <si>
+    <t>1214A9C</t>
+  </si>
+  <si>
+    <t>120EEEC</t>
+  </si>
+  <si>
+    <t>12187E8</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210DA8, 1   // Fuel Sauber</t>
+  </si>
+  <si>
+    <t>// mov     ds:dword_1210D7C, 0   // Fuel Sauber</t>
+  </si>
+  <si>
+    <t>Engine Terms</t>
+  </si>
+  <si>
+    <t>Engine Deal</t>
+  </si>
+  <si>
+    <t>Tyre Deal</t>
+  </si>
+  <si>
+    <t>Tyre Terms</t>
+  </si>
+  <si>
+    <t>Fuel Deal</t>
+  </si>
+  <si>
+    <t>Fuel Terms</t>
+  </si>
+  <si>
+    <t>TeamBaseOffset</t>
   </si>
 </sst>
 </file>
@@ -9527,15 +9851,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA8644C-41AD-4A54-BCE8-1C7AF19E30AC}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34:N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>133</v>
       </c>
@@ -9551,7 +9875,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -9567,7 +9891,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
@@ -9583,7 +9907,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>132</v>
       </c>
@@ -9599,7 +9923,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>121</v>
       </c>
@@ -9615,7 +9939,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>129</v>
       </c>
@@ -9631,7 +9955,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>123</v>
       </c>
@@ -9647,7 +9971,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>130</v>
       </c>
@@ -9663,7 +9987,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -9679,7 +10003,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>122</v>
       </c>
@@ -9695,9 +10019,893 @@
         <v>571</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>576</v>
+      </c>
+      <c r="G14">
+        <v>1209364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>577</v>
+      </c>
+      <c r="G15">
+        <v>1209338</v>
+      </c>
+      <c r="H15">
+        <f>HEX2DEC(G15)-HEX2DEC(G14)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>578</v>
+      </c>
+      <c r="G16" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>579</v>
+      </c>
+      <c r="G17" t="s">
+        <v>599</v>
+      </c>
+      <c r="H17">
+        <f>HEX2DEC(G17)-HEX2DEC(G16)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>580</v>
+      </c>
+      <c r="G18" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>581</v>
+      </c>
+      <c r="G19" t="s">
+        <v>601</v>
+      </c>
+      <c r="H19">
+        <f>HEX2DEC(G19)-HEX2DEC(G18)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>582</v>
+      </c>
+      <c r="G20" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>583</v>
+      </c>
+      <c r="G21" t="s">
+        <v>603</v>
+      </c>
+      <c r="H21">
+        <f>HEX2DEC(G21)-HEX2DEC(G20)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>584</v>
+      </c>
+      <c r="G22" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>585</v>
+      </c>
+      <c r="G23" t="s">
+        <v>605</v>
+      </c>
+      <c r="H23">
+        <f>HEX2DEC(G23)-HEX2DEC(G22)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>586</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>587</v>
+      </c>
+      <c r="G25" t="s">
+        <v>606</v>
+      </c>
+      <c r="H25">
+        <f>HEX2DEC(G25)-HEX2DEC(G24)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>588</v>
+      </c>
+      <c r="G26">
+        <v>1205644</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>589</v>
+      </c>
+      <c r="G27">
+        <v>1205618</v>
+      </c>
+      <c r="H27">
+        <f>HEX2DEC(G27)-HEX2DEC(G26)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>590</v>
+      </c>
+      <c r="G28" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>591</v>
+      </c>
+      <c r="G29" t="s">
+        <v>608</v>
+      </c>
+      <c r="H29">
+        <f>HEX2DEC(G29)-HEX2DEC(G28)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>592</v>
+      </c>
+      <c r="G30" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>593</v>
+      </c>
+      <c r="G31" t="s">
+        <v>610</v>
+      </c>
+      <c r="H31">
+        <f>HEX2DEC(G31)-HEX2DEC(G30)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>594</v>
+      </c>
+      <c r="G32" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>595</v>
+      </c>
+      <c r="G33" t="s">
+        <v>612</v>
+      </c>
+      <c r="H33">
+        <f>HEX2DEC(G33)-HEX2DEC(G32)</f>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>596</v>
+      </c>
+      <c r="G34">
+        <v>1216954</v>
+      </c>
+      <c r="L34" t="s">
+        <v>683</v>
+      </c>
+      <c r="N34">
+        <v>1205614</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>597</v>
+      </c>
+      <c r="G35">
+        <v>1216928</v>
+      </c>
+      <c r="H35">
+        <f>HEX2DEC(G35)-HEX2DEC(G34)</f>
+        <v>-44</v>
+      </c>
+      <c r="L35" t="s">
+        <v>683</v>
+      </c>
+      <c r="N35">
+        <v>7824</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>614</v>
+      </c>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36">
+        <f>HEX2DEC(G36)-HEX2DEC(G20)</f>
+        <v>-4</v>
+      </c>
+      <c r="L36" t="s">
+        <v>678</v>
+      </c>
+      <c r="N36">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>615</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37">
+        <f>HEX2DEC(G37)-HEX2DEC(G36)</f>
+        <v>-44</v>
+      </c>
+      <c r="I37">
+        <f>HEX2DEC(G37)-HEX2DEC(G21)</f>
+        <v>-4</v>
+      </c>
+      <c r="L37" t="s">
+        <v>677</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>616</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38">
+        <f>HEX2DEC(G38)-HEX2DEC(G28)</f>
+        <v>-4</v>
+      </c>
+      <c r="L38" t="s">
+        <v>679</v>
+      </c>
+      <c r="N38">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>617</v>
+      </c>
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39">
+        <f>HEX2DEC(G39)-HEX2DEC(G38)</f>
+        <v>-44</v>
+      </c>
+      <c r="I39">
+        <f>HEX2DEC(G39)-HEX2DEC(G29)</f>
+        <v>-4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>680</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>618</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40">
+        <f>HEX2DEC(G40)-HEX2DEC(G32)</f>
+        <v>-4</v>
+      </c>
+      <c r="L40" t="s">
+        <v>681</v>
+      </c>
+      <c r="N40">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>619</v>
+      </c>
+      <c r="G41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41">
+        <f>HEX2DEC(G41)-HEX2DEC(G40)</f>
+        <v>-44</v>
+      </c>
+      <c r="I41">
+        <f>HEX2DEC(G41)-HEX2DEC(G33)</f>
+        <v>-4</v>
+      </c>
+      <c r="L41" t="s">
+        <v>682</v>
+      </c>
+      <c r="N41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>620</v>
+      </c>
+      <c r="G42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42">
+        <f>HEX2DEC(G42)-HEX2DEC(G22)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>621</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <f>HEX2DEC(G43)-HEX2DEC(G42)</f>
+        <v>-44</v>
+      </c>
+      <c r="I43">
+        <f>HEX2DEC(G43)-HEX2DEC(G23)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>622</v>
+      </c>
+      <c r="G44">
+        <v>1216950</v>
+      </c>
+      <c r="I44">
+        <f>HEX2DEC(G44)-HEX2DEC(G34)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>623</v>
+      </c>
+      <c r="G45">
+        <v>1216924</v>
+      </c>
+      <c r="H45">
+        <f>HEX2DEC(G45)-HEX2DEC(G44)</f>
+        <v>-44</v>
+      </c>
+      <c r="I45">
+        <f>HEX2DEC(G45)-HEX2DEC(G35)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>624</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46">
+        <f>HEX2DEC(G46)-HEX2DEC(G24)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>625</v>
+      </c>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47">
+        <f>HEX2DEC(G47)-HEX2DEC(G46)</f>
+        <v>-44</v>
+      </c>
+      <c r="I47">
+        <f>HEX2DEC(G47)-HEX2DEC(G25)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>626</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48">
+        <f>HEX2DEC(G48)-HEX2DEC(G16)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>627</v>
+      </c>
+      <c r="G49" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49">
+        <f>HEX2DEC(G49)-HEX2DEC(G48)</f>
+        <v>-44</v>
+      </c>
+      <c r="I49">
+        <f>HEX2DEC(G49)-HEX2DEC(G17)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>628</v>
+      </c>
+      <c r="G50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I50">
+        <f>HEX2DEC(G50)-HEX2DEC(G30)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>629</v>
+      </c>
+      <c r="G51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51">
+        <f>HEX2DEC(G51)-HEX2DEC(G50)</f>
+        <v>-44</v>
+      </c>
+      <c r="I51">
+        <f>HEX2DEC(G51)-HEX2DEC(G31)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>630</v>
+      </c>
+      <c r="G52" t="s">
+        <v>62</v>
+      </c>
+      <c r="I52">
+        <f>HEX2DEC(G52)-HEX2DEC(G18)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>631</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53">
+        <f>HEX2DEC(G53)-HEX2DEC(G52)</f>
+        <v>-44</v>
+      </c>
+      <c r="I53">
+        <f>HEX2DEC(G53)-HEX2DEC(G19)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>632</v>
+      </c>
+      <c r="G54">
+        <v>1205640</v>
+      </c>
+      <c r="I54">
+        <f>HEX2DEC(G54)-HEX2DEC(G26)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>633</v>
+      </c>
+      <c r="G55">
+        <v>1205614</v>
+      </c>
+      <c r="H55">
+        <f>HEX2DEC(G55)-HEX2DEC(G54)</f>
+        <v>-44</v>
+      </c>
+      <c r="I55">
+        <f>HEX2DEC(G55)-HEX2DEC(G27)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>634</v>
+      </c>
+      <c r="G56">
+        <v>1209360</v>
+      </c>
+      <c r="I56">
+        <f>HEX2DEC(G56)-HEX2DEC(G14)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>635</v>
+      </c>
+      <c r="G57">
+        <v>1209334</v>
+      </c>
+      <c r="H57">
+        <f>HEX2DEC(G57)-HEX2DEC(G56)</f>
+        <v>-44</v>
+      </c>
+      <c r="I57">
+        <f>HEX2DEC(G57)-HEX2DEC(G15)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>636</v>
+      </c>
+      <c r="G58">
+        <v>1205648</v>
+      </c>
+      <c r="I58">
+        <f>HEX2DEC(G58)-HEX2DEC(G26)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>637</v>
+      </c>
+      <c r="G59" t="s">
+        <v>656</v>
+      </c>
+      <c r="H59">
+        <f>HEX2DEC(G59)-HEX2DEC(G58)</f>
+        <v>-44</v>
+      </c>
+      <c r="I59">
+        <f>HEX2DEC(G59)-HEX2DEC(G27)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>638</v>
+      </c>
+      <c r="G60" t="s">
+        <v>657</v>
+      </c>
+      <c r="I60">
+        <f>HEX2DEC(G60)-HEX2DEC(G28)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>639</v>
+      </c>
+      <c r="G61" t="s">
+        <v>658</v>
+      </c>
+      <c r="H61">
+        <f>HEX2DEC(G61)-HEX2DEC(G60)</f>
+        <v>-44</v>
+      </c>
+      <c r="I61">
+        <f>HEX2DEC(G61)-HEX2DEC(G29)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>675</v>
+      </c>
+      <c r="G62" t="s">
+        <v>659</v>
+      </c>
+      <c r="I62">
+        <f>HEX2DEC(G62)-HEX2DEC(G32)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>676</v>
+      </c>
+      <c r="G63" t="s">
+        <v>660</v>
+      </c>
+      <c r="H63">
+        <f>HEX2DEC(G63)-HEX2DEC(G62)</f>
+        <v>-44</v>
+      </c>
+      <c r="I63">
+        <f>HEX2DEC(G63)-HEX2DEC(G33)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>640</v>
+      </c>
+      <c r="G64">
+        <v>1209368</v>
+      </c>
+      <c r="I64">
+        <f>HEX2DEC(G64)-HEX2DEC(G14)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>641</v>
+      </c>
+      <c r="G65" t="s">
+        <v>661</v>
+      </c>
+      <c r="H65">
+        <f>HEX2DEC(G65)-HEX2DEC(G64)</f>
+        <v>-44</v>
+      </c>
+      <c r="I65">
+        <f>HEX2DEC(G65)-HEX2DEC(G15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>642</v>
+      </c>
+      <c r="G66" t="s">
+        <v>662</v>
+      </c>
+      <c r="I66">
+        <f>HEX2DEC(G66)-HEX2DEC(G16)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>643</v>
+      </c>
+      <c r="G67" t="s">
+        <v>663</v>
+      </c>
+      <c r="H67">
+        <f>HEX2DEC(G67)-HEX2DEC(G66)</f>
+        <v>-44</v>
+      </c>
+      <c r="I67">
+        <f>HEX2DEC(G67)-HEX2DEC(G17)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>644</v>
+      </c>
+      <c r="G68" t="s">
+        <v>664</v>
+      </c>
+      <c r="I68">
+        <f>HEX2DEC(G68)-HEX2DEC(G30)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>645</v>
+      </c>
+      <c r="G69" t="s">
+        <v>665</v>
+      </c>
+      <c r="H69">
+        <f>HEX2DEC(G69)-HEX2DEC(G68)</f>
+        <v>-44</v>
+      </c>
+      <c r="I69">
+        <f>HEX2DEC(G69)-HEX2DEC(G31)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>646</v>
+      </c>
+      <c r="G70" t="s">
+        <v>666</v>
+      </c>
+      <c r="I70">
+        <f>HEX2DEC(G70)-HEX2DEC(G18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>647</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="H71">
+        <f>HEX2DEC(G71)-HEX2DEC(G70)</f>
+        <v>-44</v>
+      </c>
+      <c r="I71">
+        <f>HEX2DEC(G71)-HEX2DEC(G19)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>648</v>
+      </c>
+      <c r="G72" t="s">
+        <v>667</v>
+      </c>
+      <c r="I72">
+        <f>HEX2DEC(G72)-HEX2DEC(G20)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>649</v>
+      </c>
+      <c r="G73" t="s">
+        <v>668</v>
+      </c>
+      <c r="H73">
+        <f>HEX2DEC(G73)-HEX2DEC(G72)</f>
+        <v>-44</v>
+      </c>
+      <c r="I73">
+        <f>HEX2DEC(G73)-HEX2DEC(G21)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>650</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="I74">
+        <f>HEX2DEC(G74)-HEX2DEC(G24)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>651</v>
+      </c>
+      <c r="G75" t="s">
+        <v>669</v>
+      </c>
+      <c r="H75">
+        <f>HEX2DEC(G75)-HEX2DEC(G74)</f>
+        <v>-44</v>
+      </c>
+      <c r="I75">
+        <f>HEX2DEC(G75)-HEX2DEC(G25)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>652</v>
+      </c>
+      <c r="G76">
+        <v>1216958</v>
+      </c>
+      <c r="I76">
+        <f>HEX2DEC(G76)-HEX2DEC(G34)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>653</v>
+      </c>
+      <c r="G77" t="s">
+        <v>670</v>
+      </c>
+      <c r="H77">
+        <f>HEX2DEC(G77)-HEX2DEC(G76)</f>
+        <v>-44</v>
+      </c>
+      <c r="I77">
+        <f>HEX2DEC(G77)-HEX2DEC(G35)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>654</v>
+      </c>
+      <c r="G78" t="s">
+        <v>671</v>
+      </c>
+      <c r="I78">
+        <f>HEX2DEC(G78)-HEX2DEC(G22)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>655</v>
+      </c>
+      <c r="G79" t="s">
+        <v>672</v>
+      </c>
+      <c r="H79">
+        <f>HEX2DEC(G79)-HEX2DEC(G78)</f>
+        <v>-44</v>
+      </c>
+      <c r="I79">
+        <f>HEX2DEC(G79)-HEX2DEC(G23)</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>